<commit_message>
what is the good for
</commit_message>
<xml_diff>
--- a/Buyers guide/active technology/active.com.bd.xlsx
+++ b/Buyers guide/active technology/active.com.bd.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nafees\Desktop\office\Buyers guide\active technology\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60D3ABAB-A834-4F7E-9B42-576BC68BEC7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C77D67B2-1D37-407C-911F-E2C650043EA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1014,6 +1014,30 @@
     <xf numFmtId="0" fontId="12" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1030,30 +1054,6 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1061,7 +1061,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="226">
+  <dxfs count="58">
     <dxf>
       <font>
         <b/>
@@ -1102,7 +1102,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFF0000"/>
+          <bgColor rgb="FF00FF00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1113,7 +1113,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FF00FF00"/>
+          <bgColor rgb="FFFE0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1125,1737 +1125,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFE0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFFFF"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF00FF00"/>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFFFF"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF00FF00"/>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFFFF"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF00FF00"/>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFFFF"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF00FF00"/>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFFFF"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF00FF00"/>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFFFF"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF00FF00"/>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFFFF"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF00FF00"/>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFFFF"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF00FF00"/>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFFFF"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF00FF00"/>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFFFF"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF00FF00"/>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFFFF"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF00FF00"/>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFFFF"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF00FF00"/>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFFFF"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF00FF00"/>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFE0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFFFF"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF00FF00"/>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFFFF"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF00FF00"/>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFFFF"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF00FF00"/>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFFFF"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF00FF00"/>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFFFF"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF00FF00"/>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFFFF"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF00FF00"/>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFFFF"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF00FF00"/>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFFFF"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF00FF00"/>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFFFF"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF00FF00"/>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFFFF"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF00FF00"/>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFFFF"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF00FF00"/>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFFFF"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF00FF00"/>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFFFF"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF00FF00"/>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFE0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFFFF"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF00FF00"/>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFFFF"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF00FF00"/>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFFFF"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF00FF00"/>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFFFF"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF00FF00"/>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFFFF"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF00FF00"/>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFFFF"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF00FF00"/>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFFFF"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF00FF00"/>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFFFF"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF00FF00"/>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFFFF"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF00FF00"/>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFFFF"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF00FF00"/>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFFFF"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF00FF00"/>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFFFF"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF00FF00"/>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFFFF"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFF00"/>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF00FF00"/>
-          <bgColor rgb="FF00FF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFF0000"/>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF00"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFE0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00FF00"/>
         </patternFill>
       </fill>
     </dxf>
@@ -3677,30 +1946,30 @@
   <dimension ref="A1:I980"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B49" sqref="B49"/>
+      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I52" sqref="I52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="11" style="1" customWidth="1"/>
-    <col min="2" max="2" width="19.42578125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" style="1" customWidth="1"/>
     <col min="3" max="3" width="11.85546875" style="1" customWidth="1"/>
     <col min="4" max="4" width="23" style="1" customWidth="1"/>
-    <col min="5" max="5" width="30.5703125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="26.42578125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="17.5703125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="11" style="1" customWidth="1"/>
-    <col min="9" max="9" width="20.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="30.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="21.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="12.140625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="9.85546875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="13.42578125" style="1" customWidth="1"/>
     <col min="10" max="10" width="17.28515625" style="1" customWidth="1"/>
     <col min="11" max="16384" width="14.42578125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="25.5" customHeight="1">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="58" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="48"/>
+      <c r="B1" s="56"/>
       <c r="C1" s="38" t="s">
         <v>37</v>
       </c>
@@ -3714,16 +1983,16 @@
         <v>2</v>
       </c>
       <c r="G1" s="40"/>
-      <c r="H1" s="51" t="s">
+      <c r="H1" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="48"/>
-    </row>
-    <row r="2" spans="1:9" ht="12.75">
-      <c r="A2" s="52" t="s">
+      <c r="I1" s="56"/>
+    </row>
+    <row r="2" spans="1:9" ht="16.5" customHeight="1">
+      <c r="A2" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="48"/>
+      <c r="B2" s="56"/>
       <c r="C2" s="5"/>
       <c r="D2" s="3" t="s">
         <v>5</v>
@@ -3742,8 +2011,8 @@
       </c>
     </row>
     <row r="3" spans="1:9" ht="18" customHeight="1">
-      <c r="A3" s="52"/>
-      <c r="B3" s="48"/>
+      <c r="A3" s="60"/>
+      <c r="B3" s="56"/>
       <c r="C3" s="5"/>
       <c r="D3" s="7" t="s">
         <v>8</v>
@@ -3766,10 +2035,10 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="25.5" customHeight="1">
-      <c r="A4" s="52" t="s">
+      <c r="A4" s="60" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="48"/>
+      <c r="B4" s="56"/>
       <c r="C4" s="5"/>
       <c r="D4" s="7" t="s">
         <v>12</v>
@@ -3792,15 +2061,15 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="18" customHeight="1">
-      <c r="A5" s="47" t="s">
+      <c r="A5" s="55" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="48"/>
-      <c r="C5" s="47"/>
-      <c r="D5" s="49"/>
-      <c r="E5" s="49"/>
-      <c r="F5" s="49"/>
-      <c r="G5" s="48"/>
+      <c r="B5" s="56"/>
+      <c r="C5" s="55"/>
+      <c r="D5" s="57"/>
+      <c r="E5" s="57"/>
+      <c r="F5" s="57"/>
+      <c r="G5" s="56"/>
       <c r="H5" s="10" t="s">
         <v>16</v>
       </c>
@@ -3835,7 +2104,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="33.75" customHeight="1">
+    <row r="7" spans="1:9" ht="24.75" customHeight="1">
       <c r="A7" s="33" t="s">
         <v>25</v>
       </c>
@@ -3855,7 +2124,7 @@
       <c r="G7" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="53"/>
+      <c r="H7" s="47"/>
     </row>
     <row r="8" spans="1:9" ht="26.25" customHeight="1">
       <c r="A8" s="13" t="s">
@@ -3877,7 +2146,7 @@
       <c r="G8" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="H8" s="53" t="s">
+      <c r="H8" s="47" t="s">
         <v>45</v>
       </c>
     </row>
@@ -3901,7 +2170,7 @@
       <c r="G9" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="H9" s="53" t="s">
+      <c r="H9" s="47" t="s">
         <v>48</v>
       </c>
     </row>
@@ -3925,7 +2194,7 @@
       <c r="G10" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="H10" s="53"/>
+      <c r="H10" s="47"/>
     </row>
     <row r="11" spans="1:9" ht="25.5" customHeight="1">
       <c r="A11" s="37" t="s">
@@ -3947,7 +2216,7 @@
       <c r="G11" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="H11" s="54" t="s">
+      <c r="H11" s="48" t="s">
         <v>56</v>
       </c>
     </row>
@@ -3971,7 +2240,7 @@
       <c r="G12" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="H12" s="54"/>
+      <c r="H12" s="48"/>
     </row>
     <row r="13" spans="1:9" ht="30.75" customHeight="1">
       <c r="A13" s="33" t="s">
@@ -3993,9 +2262,9 @@
       <c r="G13" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="H13" s="55"/>
-    </row>
-    <row r="14" spans="1:9" ht="25.5" customHeight="1">
+      <c r="H13" s="49"/>
+    </row>
+    <row r="14" spans="1:9" ht="24" customHeight="1">
       <c r="A14" s="42" t="s">
         <v>33</v>
       </c>
@@ -4085,7 +2354,7 @@
       </c>
       <c r="H17" s="25"/>
     </row>
-    <row r="18" spans="1:8" ht="53.25" customHeight="1">
+    <row r="18" spans="1:8" ht="54.75" customHeight="1">
       <c r="A18" s="13" t="s">
         <v>75</v>
       </c>
@@ -4107,7 +2376,7 @@
       </c>
       <c r="H18" s="23"/>
     </row>
-    <row r="19" spans="1:8" ht="39" customHeight="1">
+    <row r="19" spans="1:8" ht="53.25" customHeight="1">
       <c r="A19" s="13" t="s">
         <v>77</v>
       </c>
@@ -4131,7 +2400,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="73.5" customHeight="1">
+    <row r="20" spans="1:8" ht="62.25" customHeight="1">
       <c r="A20" s="21" t="s">
         <v>78</v>
       </c>
@@ -4153,7 +2422,7 @@
       </c>
       <c r="H20" s="23"/>
     </row>
-    <row r="21" spans="1:8" ht="34.5" customHeight="1">
+    <row r="21" spans="1:8" ht="33" customHeight="1">
       <c r="A21" s="33" t="s">
         <v>82</v>
       </c>
@@ -4173,7 +2442,7 @@
       <c r="G21" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="H21" s="56" t="s">
+      <c r="H21" s="50" t="s">
         <v>68</v>
       </c>
     </row>
@@ -4197,7 +2466,7 @@
       <c r="G22" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="H22" s="57" t="s">
+      <c r="H22" s="51" t="s">
         <v>92</v>
       </c>
     </row>
@@ -4245,7 +2514,7 @@
       </c>
       <c r="H24" s="23"/>
     </row>
-    <row r="25" spans="1:8" ht="21" customHeight="1">
+    <row r="25" spans="1:8" ht="17.25" customHeight="1">
       <c r="A25" s="33" t="s">
         <v>96</v>
       </c>
@@ -4267,7 +2536,7 @@
       </c>
       <c r="H25" s="25"/>
     </row>
-    <row r="26" spans="1:8" ht="66.75" customHeight="1">
+    <row r="26" spans="1:8" ht="63" customHeight="1">
       <c r="A26" s="42" t="s">
         <v>98</v>
       </c>
@@ -4289,7 +2558,7 @@
       </c>
       <c r="H26" s="23"/>
     </row>
-    <row r="27" spans="1:8" ht="75.75" customHeight="1">
+    <row r="27" spans="1:8" ht="76.5" customHeight="1">
       <c r="A27" s="33" t="s">
         <v>101</v>
       </c>
@@ -4311,7 +2580,7 @@
       </c>
       <c r="H27" s="23"/>
     </row>
-    <row r="28" spans="1:8" ht="35.25" customHeight="1">
+    <row r="28" spans="1:8" ht="30" customHeight="1">
       <c r="A28" s="33" t="s">
         <v>107</v>
       </c>
@@ -4333,7 +2602,7 @@
       </c>
       <c r="H28" s="25"/>
     </row>
-    <row r="29" spans="1:8" ht="30.75" customHeight="1">
+    <row r="29" spans="1:8" ht="27.75" customHeight="1">
       <c r="A29" s="42" t="s">
         <v>109</v>
       </c>
@@ -4397,7 +2666,7 @@
       <c r="G31" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="H31" s="57" t="s">
+      <c r="H31" s="51" t="s">
         <v>68</v>
       </c>
     </row>
@@ -4423,7 +2692,7 @@
       </c>
       <c r="H32" s="23"/>
     </row>
-    <row r="33" spans="1:8" ht="78" customHeight="1">
+    <row r="33" spans="1:8" ht="78.75" customHeight="1">
       <c r="A33" s="33" t="s">
         <v>119</v>
       </c>
@@ -4445,7 +2714,7 @@
       </c>
       <c r="H33" s="23"/>
     </row>
-    <row r="34" spans="1:8" ht="43.5" customHeight="1">
+    <row r="34" spans="1:8" ht="37.5" customHeight="1">
       <c r="A34" s="33" t="s">
         <v>122</v>
       </c>
@@ -4467,7 +2736,7 @@
       </c>
       <c r="H34" s="25"/>
     </row>
-    <row r="35" spans="1:8" ht="87" customHeight="1">
+    <row r="35" spans="1:8" ht="79.5" customHeight="1">
       <c r="A35" s="42" t="s">
         <v>126</v>
       </c>
@@ -4641,7 +2910,7 @@
       <c r="G42" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="H42" s="56" t="s">
+      <c r="H42" s="50" t="s">
         <v>151</v>
       </c>
     </row>
@@ -4652,7 +2921,7 @@
       <c r="B43" s="35" t="s">
         <v>153</v>
       </c>
-      <c r="C43" s="58" t="s">
+      <c r="C43" s="52" t="s">
         <v>154</v>
       </c>
       <c r="D43" s="34" t="s">
@@ -4667,7 +2936,7 @@
       <c r="G43" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="H43" s="57" t="s">
+      <c r="H43" s="51" t="s">
         <v>156</v>
       </c>
     </row>
@@ -4678,7 +2947,7 @@
       <c r="B44" s="34" t="s">
         <v>153</v>
       </c>
-      <c r="C44" s="59" t="s">
+      <c r="C44" s="53" t="s">
         <v>159</v>
       </c>
       <c r="D44" s="35" t="s">
@@ -4693,7 +2962,7 @@
       <c r="G44" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="H44" s="56" t="s">
+      <c r="H44" s="50" t="s">
         <v>161</v>
       </c>
     </row>
@@ -4704,7 +2973,7 @@
       <c r="B45" s="35" t="s">
         <v>153</v>
       </c>
-      <c r="C45" s="60" t="s">
+      <c r="C45" s="54" t="s">
         <v>163</v>
       </c>
       <c r="D45" s="35" t="s">
@@ -4719,7 +2988,7 @@
       <c r="G45" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="H45" s="56" t="s">
+      <c r="H45" s="50" t="s">
         <v>166</v>
       </c>
     </row>
@@ -4799,86 +3068,14 @@
       <c r="G49" s="16"/>
       <c r="H49" s="23"/>
     </row>
-    <row r="50" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A50" s="13"/>
-      <c r="B50" s="14"/>
-      <c r="C50" s="22"/>
-      <c r="D50" s="14"/>
-      <c r="E50" s="14"/>
-      <c r="F50" s="16"/>
-      <c r="G50" s="16"/>
-      <c r="H50" s="23"/>
-    </row>
-    <row r="51" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A51" s="13"/>
-      <c r="B51" s="14"/>
-      <c r="C51" s="22"/>
-      <c r="D51" s="14"/>
-      <c r="E51" s="14"/>
-      <c r="F51" s="16"/>
-      <c r="G51" s="16"/>
-      <c r="H51" s="23"/>
-    </row>
-    <row r="52" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A52" s="13"/>
-      <c r="B52" s="14"/>
-      <c r="C52" s="22"/>
-      <c r="D52" s="14"/>
-      <c r="E52" s="14"/>
-      <c r="F52" s="16"/>
-      <c r="G52" s="16"/>
-      <c r="H52" s="23"/>
-    </row>
-    <row r="53" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A53" s="13"/>
-      <c r="B53" s="14"/>
-      <c r="C53" s="22"/>
-      <c r="D53" s="14"/>
-      <c r="E53" s="14"/>
-      <c r="F53" s="16"/>
-      <c r="G53" s="16"/>
-      <c r="H53" s="23"/>
-    </row>
-    <row r="54" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A54" s="13"/>
-      <c r="B54" s="14"/>
-      <c r="C54" s="22"/>
-      <c r="D54" s="14"/>
-      <c r="E54" s="14"/>
-      <c r="F54" s="16"/>
-      <c r="G54" s="16"/>
-      <c r="H54" s="23"/>
-    </row>
-    <row r="55" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A55" s="13"/>
-      <c r="B55" s="14"/>
-      <c r="C55" s="22"/>
-      <c r="D55" s="14"/>
-      <c r="E55" s="14"/>
-      <c r="F55" s="16"/>
-      <c r="G55" s="16"/>
-      <c r="H55" s="23"/>
-    </row>
-    <row r="56" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A56" s="13"/>
-      <c r="B56" s="14"/>
-      <c r="C56" s="22"/>
-      <c r="D56" s="14"/>
-      <c r="E56" s="14"/>
-      <c r="F56" s="16"/>
-      <c r="G56" s="16"/>
-      <c r="H56" s="23"/>
-    </row>
-    <row r="57" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A57" s="13"/>
-      <c r="B57" s="14"/>
-      <c r="C57" s="22"/>
-      <c r="D57" s="14"/>
-      <c r="E57" s="14"/>
-      <c r="F57" s="16"/>
-      <c r="G57" s="16"/>
-      <c r="H57" s="23"/>
-    </row>
+    <row r="50" spans="1:8" ht="15.75" customHeight="1"/>
+    <row r="51" spans="1:8" ht="15.75" customHeight="1"/>
+    <row r="52" spans="1:8" ht="15.75" customHeight="1"/>
+    <row r="53" spans="1:8" ht="15.75" customHeight="1"/>
+    <row r="54" spans="1:8" ht="15.75" customHeight="1"/>
+    <row r="55" spans="1:8" ht="15.75" customHeight="1"/>
+    <row r="56" spans="1:8" ht="15.75" customHeight="1"/>
+    <row r="57" spans="1:8" ht="15.75" customHeight="1"/>
     <row r="58" spans="1:8" ht="15.75" customHeight="1"/>
     <row r="59" spans="1:8" ht="15.75" customHeight="1"/>
     <row r="60" spans="1:8" ht="15.75" customHeight="1"/>
@@ -5814,207 +4011,207 @@
   </mergeCells>
   <phoneticPr fontId="15" type="noConversion"/>
   <conditionalFormatting sqref="I2">
-    <cfRule type="cellIs" dxfId="114" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="57" priority="31" operator="equal">
       <formula>"FAIL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="113" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="32" operator="equal">
       <formula>"PASS"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="112" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="33" operator="equal">
       <formula>"WARNING"</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="111" priority="34">
+    <cfRule type="containsBlanks" dxfId="54" priority="34">
       <formula>LEN(TRIM(I2))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I3">
-    <cfRule type="cellIs" dxfId="110" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="53" priority="27" operator="equal">
       <formula>"FAIL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="109" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="52" priority="28" operator="equal">
       <formula>"PASS"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="108" priority="29" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="29" operator="equal">
       <formula>"WARNING"</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="107" priority="30">
+    <cfRule type="containsBlanks" dxfId="50" priority="30">
       <formula>LEN(TRIM(I3))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G7">
-    <cfRule type="cellIs" dxfId="106" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="49" priority="23" operator="equal">
       <formula>"FAIL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="105" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="48" priority="24" operator="equal">
       <formula>"PASS"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="104" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="25" operator="equal">
       <formula>"WARNING"</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="103" priority="26">
+    <cfRule type="containsBlanks" dxfId="46" priority="26">
       <formula>LEN(TRIM(G7))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G19">
-    <cfRule type="cellIs" dxfId="102" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="45" priority="19" operator="equal">
       <formula>"FAIL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="101" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="44" priority="20" operator="equal">
       <formula>"PASS"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="100" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="21" operator="equal">
       <formula>"WARNING"</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="99" priority="22">
+    <cfRule type="containsBlanks" dxfId="42" priority="22">
       <formula>LEN(TRIM(G19))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G25">
-    <cfRule type="cellIs" dxfId="98" priority="51" operator="equal">
+    <cfRule type="cellIs" dxfId="41" priority="51" operator="equal">
       <formula>"FAIL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="97" priority="52" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="52" operator="equal">
       <formula>"PASS"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="96" priority="53" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="53" operator="equal">
       <formula>"WARNING"</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="95" priority="54">
+    <cfRule type="containsBlanks" dxfId="38" priority="54">
       <formula>LEN(TRIM(G25))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G28">
-    <cfRule type="cellIs" dxfId="94" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="47" operator="equal">
       <formula>"FAIL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="93" priority="48" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="48" operator="equal">
       <formula>"PASS"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="92" priority="49" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="49" operator="equal">
       <formula>"WARNING"</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="91" priority="50">
+    <cfRule type="containsBlanks" dxfId="34" priority="50">
       <formula>LEN(TRIM(G28))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G31">
-    <cfRule type="cellIs" dxfId="90" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="15" operator="equal">
       <formula>"FAIL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="89" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="32" priority="16" operator="equal">
       <formula>"PASS"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="88" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="31" priority="17" operator="equal">
       <formula>"WARNING"</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="87" priority="18">
+    <cfRule type="containsBlanks" dxfId="30" priority="18">
       <formula>LEN(TRIM(G31))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G34">
-    <cfRule type="cellIs" dxfId="86" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="43" operator="equal">
       <formula>"FAIL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="85" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="44" operator="equal">
       <formula>"PASS"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="84" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="45" operator="equal">
       <formula>"WARNING"</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="83" priority="46">
+    <cfRule type="containsBlanks" dxfId="26" priority="46">
       <formula>LEN(TRIM(G34))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G37">
-    <cfRule type="cellIs" dxfId="82" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="39" operator="equal">
       <formula>"FAIL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="81" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="24" priority="40" operator="equal">
       <formula>"PASS"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="80" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="23" priority="41" operator="equal">
       <formula>"WARNING"</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="79" priority="42">
+    <cfRule type="containsBlanks" dxfId="22" priority="42">
       <formula>LEN(TRIM(G37))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G40">
-    <cfRule type="cellIs" dxfId="78" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="35" operator="equal">
       <formula>"FAIL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="77" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="36" operator="equal">
       <formula>"PASS"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="76" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="37" operator="equal">
       <formula>"WARNING"</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="75" priority="38">
+    <cfRule type="containsBlanks" dxfId="18" priority="38">
       <formula>LEN(TRIM(G40))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G43">
-    <cfRule type="cellIs" dxfId="74" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="11" operator="equal">
       <formula>"FAIL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="73" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="12" operator="equal">
       <formula>"PASS"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="72" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="13" operator="equal">
       <formula>"WARNING"</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="71" priority="14">
+    <cfRule type="containsBlanks" dxfId="14" priority="14">
       <formula>LEN(TRIM(G43))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G46">
-    <cfRule type="cellIs" dxfId="70" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="7" operator="equal">
       <formula>"FAIL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="69" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="8" operator="equal">
       <formula>"PASS"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="68" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="9" operator="equal">
       <formula>"WARNING"</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="67" priority="10">
+    <cfRule type="containsBlanks" dxfId="10" priority="10">
       <formula>LEN(TRIM(G46))=0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G10 G22 G8 G16 G13">
-    <cfRule type="cellIs" dxfId="66" priority="55" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="55" operator="equal">
       <formula>"FAIL"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="65" priority="56" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="56" operator="equal">
       <formula>"PASS"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="57" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="57" operator="equal">
       <formula>"WARNING"</formula>
     </cfRule>
-    <cfRule type="containsBlanks" dxfId="63" priority="58">
+    <cfRule type="containsBlanks" dxfId="6" priority="58">
       <formula>LEN(TRIM(G8))=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G7:G57">
-    <cfRule type="containsText" dxfId="62" priority="6" operator="containsText" text="PASS">
+  <conditionalFormatting sqref="G7:G49">
+    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="WARNING">
+      <formula>NOT(ISERROR(SEARCH("WARNING",G7)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="5" operator="containsText" text="FAIL">
+      <formula>NOT(ISERROR(SEARCH("FAIL",G7)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",G7)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="61" priority="5" operator="containsText" text="FAIL">
-      <formula>NOT(ISERROR(SEARCH("FAIL",G7)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="60" priority="4" operator="containsText" text="WARNING">
-      <formula>NOT(ISERROR(SEARCH("WARNING",G7)))</formula>
-    </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G48:G57">
+  <conditionalFormatting sqref="G48:G49">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="WARNING">
+      <formula>NOT(ISERROR(SEARCH("WARNING",G48)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="FAIL">
+      <formula>NOT(ISERROR(SEARCH("FAIL",G48)))</formula>
+    </cfRule>
     <cfRule type="containsText" dxfId="0" priority="3" operator="containsText" text="PASS">
       <formula>NOT(ISERROR(SEARCH("PASS",G48)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="FAIL">
-      <formula>NOT(ISERROR(SEARCH("FAIL",G48)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="WARNING">
-      <formula>NOT(ISERROR(SEARCH("WARNING",G48)))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
@@ -6023,6 +4220,6 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape" r:id="rId1"/>
+  <pageSetup scale="80" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>